<commit_message>
Correção na númeração das apostilas
</commit_message>
<xml_diff>
--- a/MEPIJU-QUÍMICA.xlsx
+++ b/MEPIJU-QUÍMICA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conat\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conat\Desktop\Apostilas Mepi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94645A7-DB7A-47C2-8AA7-DB65447F3613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C1181C4-7141-4F4B-9EC3-1E3AC0390778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,10 +262,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -281,9 +277,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +506,7 @@
   <dimension ref="A1:C1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -527,225 +527,225 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="9"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>

</xml_diff>